<commit_message>
update  Please enter the commit message for your changes. Lines starting
</commit_message>
<xml_diff>
--- a/Evaluation Construire le schema entité association/Dictionnaire de données.xlsx
+++ b/Evaluation Construire le schema entité association/Dictionnaire de données.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
   <si>
     <t>Code</t>
   </si>
@@ -156,7 +156,10 @@
     <t>user_id</t>
   </si>
   <si>
-    <t>v</t>
+    <t>numéro de semaine</t>
+  </si>
+  <si>
+    <t>week_id</t>
   </si>
 </sst>
 </file>
@@ -208,8 +211,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="D3:G22" totalsRowShown="0">
-  <autoFilter ref="D3:G22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="D3:G28" totalsRowShown="0">
+  <autoFilter ref="D3:G28">
     <filterColumn colId="3"/>
   </autoFilter>
   <tableColumns count="4">
@@ -507,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:G22"/>
+  <dimension ref="B3:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -547,9 +550,6 @@
       <c r="F4" t="s">
         <v>24</v>
       </c>
-      <c r="G4" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="5" spans="4:7">
       <c r="D5" t="s">
@@ -561,9 +561,6 @@
       <c r="F5" t="s">
         <v>4</v>
       </c>
-      <c r="G5" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="6" spans="4:7">
       <c r="D6" t="s">
@@ -575,9 +572,6 @@
       <c r="F6" t="s">
         <v>4</v>
       </c>
-      <c r="G6" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="7" spans="4:7">
       <c r="D7" t="s">
@@ -589,9 +583,6 @@
       <c r="F7" t="s">
         <v>4</v>
       </c>
-      <c r="G7" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="8" spans="4:7">
       <c r="D8" t="s">
@@ -603,9 +594,6 @@
       <c r="F8" t="s">
         <v>12</v>
       </c>
-      <c r="G8" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="9" spans="4:7">
       <c r="D9" t="s">
@@ -617,9 +605,6 @@
       <c r="F9" t="s">
         <v>15</v>
       </c>
-      <c r="G9" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="10" spans="4:7">
       <c r="D10" t="s">
@@ -628,9 +613,6 @@
       <c r="E10" t="s">
         <v>29</v>
       </c>
-      <c r="G10" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="11" spans="4:7">
       <c r="D11" t="s">
@@ -642,9 +624,6 @@
       <c r="F11" t="s">
         <v>4</v>
       </c>
-      <c r="G11" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="12" spans="4:7">
       <c r="D12" t="s">
@@ -656,9 +635,6 @@
       <c r="F12" t="s">
         <v>4</v>
       </c>
-      <c r="G12" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="13" spans="4:7">
       <c r="D13" t="s">
@@ -670,9 +646,6 @@
       <c r="F13" t="s">
         <v>4</v>
       </c>
-      <c r="G13" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="14" spans="4:7">
       <c r="D14" t="s">
@@ -684,9 +657,6 @@
       <c r="F14" t="s">
         <v>24</v>
       </c>
-      <c r="G14" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="15" spans="4:7">
       <c r="D15" t="s">
@@ -698,9 +668,6 @@
       <c r="F15" t="s">
         <v>4</v>
       </c>
-      <c r="G15" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="16" spans="4:7">
       <c r="D16" t="s">
@@ -712,9 +679,6 @@
       <c r="F16" t="s">
         <v>15</v>
       </c>
-      <c r="G16" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="17" spans="4:7">
       <c r="D17" t="s">
@@ -782,6 +746,24 @@
         <v>15</v>
       </c>
       <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="4:7">
+      <c r="D23" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="28" spans="4:7">
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>